<commit_message>
Graphics boosted, some text added, list of tables and graphics added
</commit_message>
<xml_diff>
--- a/Bootstrap_wyniki.xlsx
+++ b/Bootstrap_wyniki.xlsx
@@ -197,8 +197,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -433,18 +433,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -457,7 +448,7 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -466,13 +457,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -481,14 +472,8 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -496,16 +481,7 @@
     <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -516,6 +492,57 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -523,33 +550,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -898,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L72" sqref="L72"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -920,79 +920,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="38"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="47"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="H3" s="6" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="H3" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="9" t="s">
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="N4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1016,7 +1016,7 @@
         <v>56</v>
       </c>
       <c r="G5" s="2"/>
-      <c r="H5" s="19">
+      <c r="H5" s="16">
         <v>27.021000000000001</v>
       </c>
       <c r="I5" s="4">
@@ -1031,13 +1031,13 @@
       <c r="L5" s="4">
         <v>51.872999999999998</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="15">
         <v>1.1850000000000001</v>
       </c>
-      <c r="N5" s="18">
+      <c r="N5" s="15">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="O5" s="18" t="s">
+      <c r="O5" s="15" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1061,7 +1061,7 @@
         <v>238</v>
       </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="19">
+      <c r="H6" s="16">
         <v>113.06</v>
       </c>
       <c r="I6" s="4">
@@ -1076,13 +1076,13 @@
       <c r="L6" s="4">
         <v>217.99</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="15">
         <v>7.4619999999999997</v>
       </c>
-      <c r="N6" s="18">
+      <c r="N6" s="15">
         <v>0.113</v>
       </c>
-      <c r="O6" s="18" t="s">
+      <c r="O6" s="15" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1106,7 +1106,7 @@
         <v>113</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="19">
+      <c r="H7" s="16">
         <v>43.69</v>
       </c>
       <c r="I7" s="4">
@@ -1121,13 +1121,13 @@
       <c r="L7" s="4">
         <v>98.21</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="15">
         <v>3.1360000000000001</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="15">
         <v>0.28799999999999998</v>
       </c>
-      <c r="O7" s="18" t="s">
+      <c r="O7" s="15" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1167,30 +1167,30 @@
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="10" t="s">
         <v>31</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="K10" s="10" t="s">
         <v>31</v>
       </c>
       <c r="L10" s="2"/>
@@ -1208,7 +1208,7 @@
       <c r="D11" s="5">
         <v>33</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="12">
         <v>0.30780000000000002</v>
       </c>
       <c r="F11" s="2"/>
@@ -1222,7 +1222,7 @@
       <c r="J11" s="5">
         <v>808</v>
       </c>
-      <c r="K11" s="14" t="s">
+      <c r="K11" s="11" t="s">
         <v>34</v>
       </c>
       <c r="L11" s="2"/>
@@ -1249,35 +1249,35 @@
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="10" t="s">
         <v>31</v>
       </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="13" t="s">
+      <c r="L13" s="10" t="s">
         <v>31</v>
       </c>
       <c r="M13" s="2"/>
@@ -1297,7 +1297,7 @@
       <c r="E14" s="5">
         <v>23</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="12">
         <v>0.18340000000000001</v>
       </c>
       <c r="G14" s="2"/>
@@ -1313,7 +1313,7 @@
       <c r="K14" s="5">
         <v>580</v>
       </c>
-      <c r="L14" s="14" t="s">
+      <c r="L14" s="11" t="s">
         <v>33</v>
       </c>
       <c r="M14" s="2"/>
@@ -1339,30 +1339,30 @@
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="10" t="s">
         <v>31</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="13" t="s">
+      <c r="K16" s="10" t="s">
         <v>31</v>
       </c>
       <c r="L16" s="2"/>
@@ -1379,7 +1379,7 @@
       <c r="D17" s="5">
         <v>20</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="12">
         <v>0.26989999999999997</v>
       </c>
       <c r="F17" s="2"/>
@@ -1393,7 +1393,7 @@
       <c r="J17" s="5">
         <v>484</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="K17" s="11" t="s">
         <v>32</v>
       </c>
       <c r="L17" s="2"/>
@@ -1474,82 +1474,82 @@
       <c r="J22" s="40"/>
       <c r="K22" s="40"/>
       <c r="L22" s="41"/>
-      <c r="M22" s="17" t="s">
+      <c r="M22" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="H25" s="6" t="s">
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="H25" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="9" t="s">
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H26" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I26" s="7" t="s">
+      <c r="I26" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J26" s="7" t="s">
+      <c r="J26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K26" s="7" t="s">
+      <c r="K26" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L26" s="7" t="s">
+      <c r="L26" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M26" s="11" t="s">
+      <c r="M26" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="N26" s="11" t="s">
+      <c r="N26" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O26" s="11" t="s">
+      <c r="O26" s="8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1573,7 +1573,7 @@
         <v>36</v>
       </c>
       <c r="G27" s="2"/>
-      <c r="H27" s="21">
+      <c r="H27" s="18">
         <v>27.87</v>
       </c>
       <c r="I27" s="4">
@@ -1588,13 +1588,13 @@
       <c r="L27" s="4">
         <v>35.56</v>
       </c>
-      <c r="M27" s="20">
+      <c r="M27" s="17">
         <v>1.7769999999999999</v>
       </c>
-      <c r="N27" s="20">
+      <c r="N27" s="17">
         <v>0.40200000000000002</v>
       </c>
-      <c r="O27" s="20" t="s">
+      <c r="O27" s="17" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1618,7 +1618,7 @@
         <v>238</v>
       </c>
       <c r="G28" s="2"/>
-      <c r="H28" s="21">
+      <c r="H28" s="18">
         <v>108.01</v>
       </c>
       <c r="I28" s="4">
@@ -1633,13 +1633,13 @@
       <c r="L28" s="4">
         <v>217.15</v>
       </c>
-      <c r="M28" s="20">
+      <c r="M28" s="17">
         <v>18.93</v>
       </c>
-      <c r="N28" s="20">
+      <c r="N28" s="17">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="O28" s="20" t="s">
+      <c r="O28" s="17" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1663,7 +1663,7 @@
         <v>113</v>
       </c>
       <c r="G29" s="2"/>
-      <c r="H29" s="21">
+      <c r="H29" s="18">
         <v>45.17</v>
       </c>
       <c r="I29" s="4">
@@ -1678,13 +1678,13 @@
       <c r="L29" s="4">
         <v>95.53</v>
       </c>
-      <c r="M29" s="20">
+      <c r="M29" s="17">
         <v>6.8040000000000003</v>
       </c>
-      <c r="N29" s="20">
+      <c r="N29" s="17">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="O29" s="20" t="s">
+      <c r="O29" s="17" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1724,30 +1724,30 @@
       <c r="A32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="E32" s="10" t="s">
         <v>31</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I32" s="8" t="s">
+      <c r="I32" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J32" s="8" t="s">
+      <c r="J32" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K32" s="13" t="s">
+      <c r="K32" s="10" t="s">
         <v>31</v>
       </c>
       <c r="L32" s="2"/>
@@ -1765,7 +1765,7 @@
       <c r="D33" s="5">
         <v>11</v>
       </c>
-      <c r="E33" s="15"/>
+      <c r="E33" s="12"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="5">
@@ -1777,7 +1777,7 @@
       <c r="J33" s="5">
         <v>910</v>
       </c>
-      <c r="K33" s="14" t="s">
+      <c r="K33" s="11" t="s">
         <v>55</v>
       </c>
       <c r="L33" s="2"/>
@@ -1804,35 +1804,35 @@
       <c r="A35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F35" s="13" t="s">
+      <c r="F35" s="10" t="s">
         <v>31</v>
       </c>
       <c r="G35" s="2"/>
-      <c r="H35" s="8" t="s">
+      <c r="H35" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I35" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="J35" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K35" s="8" t="s">
+      <c r="K35" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L35" s="13" t="s">
+      <c r="L35" s="10" t="s">
         <v>31</v>
       </c>
       <c r="M35" s="2"/>
@@ -1852,7 +1852,7 @@
       <c r="E36" s="5">
         <v>5</v>
       </c>
-      <c r="F36" s="15"/>
+      <c r="F36" s="12"/>
       <c r="G36" s="2"/>
       <c r="H36" s="5">
         <v>166</v>
@@ -1866,7 +1866,7 @@
       <c r="K36" s="5">
         <v>417</v>
       </c>
-      <c r="L36" s="14" t="s">
+      <c r="L36" s="11" t="s">
         <v>56</v>
       </c>
       <c r="M36" s="2"/>
@@ -1892,30 +1892,30 @@
       <c r="A38" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E38" s="13" t="s">
+      <c r="E38" s="10" t="s">
         <v>31</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-      <c r="H38" s="8" t="s">
+      <c r="H38" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I38" s="8" t="s">
+      <c r="I38" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J38" s="8" t="s">
+      <c r="J38" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K38" s="13" t="s">
+      <c r="K38" s="10" t="s">
         <v>31</v>
       </c>
       <c r="L38" s="2"/>
@@ -1932,7 +1932,7 @@
       <c r="D39" s="5">
         <v>5</v>
       </c>
-      <c r="E39" s="15"/>
+      <c r="E39" s="12"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="5">
@@ -1944,7 +1944,7 @@
       <c r="J39" s="5">
         <v>412</v>
       </c>
-      <c r="K39" s="14" t="s">
+      <c r="K39" s="11" t="s">
         <v>57</v>
       </c>
       <c r="L39" s="2"/>
@@ -1981,82 +1981,82 @@
       <c r="J43" s="43"/>
       <c r="K43" s="43"/>
       <c r="L43" s="44"/>
-      <c r="M43" s="22" t="s">
+      <c r="M43" s="19" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
-      <c r="I44" s="16"/>
-      <c r="J44" s="16"/>
-      <c r="K44" s="16"/>
-      <c r="L44" s="16"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="H46" s="6" t="s">
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+      <c r="H46" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
-      <c r="M46" s="9" t="s">
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
+      <c r="K46" s="31"/>
+      <c r="L46" s="31"/>
+      <c r="M46" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="N46" s="10"/>
-      <c r="O46" s="10"/>
+      <c r="N46" s="33"/>
+      <c r="O46" s="33"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="E47" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="F47" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H47" s="7" t="s">
+      <c r="H47" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I47" s="7" t="s">
+      <c r="I47" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J47" s="7" t="s">
+      <c r="J47" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K47" s="7" t="s">
+      <c r="K47" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L47" s="7" t="s">
+      <c r="L47" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M47" s="11" t="s">
+      <c r="M47" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="N47" s="11" t="s">
+      <c r="N47" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O47" s="11" t="s">
+      <c r="O47" s="8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2080,7 +2080,7 @@
         <v>56</v>
       </c>
       <c r="G48" s="2"/>
-      <c r="H48" s="12">
+      <c r="H48" s="9">
         <v>26.68</v>
       </c>
       <c r="I48" s="4">
@@ -2095,13 +2095,13 @@
       <c r="L48" s="4">
         <v>51.86</v>
       </c>
-      <c r="M48" s="23">
+      <c r="M48" s="20">
         <v>1.49</v>
       </c>
-      <c r="N48" s="23">
+      <c r="N48" s="20">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="O48" s="23" t="s">
+      <c r="O48" s="20" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2125,7 +2125,7 @@
         <v>186</v>
       </c>
       <c r="G49" s="2"/>
-      <c r="H49" s="12">
+      <c r="H49" s="9">
         <v>114.71</v>
       </c>
       <c r="I49" s="4">
@@ -2140,13 +2140,13 @@
       <c r="L49" s="4">
         <v>179.59</v>
       </c>
-      <c r="M49" s="23">
+      <c r="M49" s="20">
         <v>7.32</v>
       </c>
-      <c r="N49" s="23">
+      <c r="N49" s="20">
         <v>0.33300000000000002</v>
       </c>
-      <c r="O49" s="23" t="s">
+      <c r="O49" s="20" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2170,7 +2170,7 @@
         <v>80</v>
       </c>
       <c r="G50" s="2"/>
-      <c r="H50" s="12">
+      <c r="H50" s="9">
         <v>43.4</v>
       </c>
       <c r="I50" s="4">
@@ -2185,13 +2185,13 @@
       <c r="L50" s="4">
         <v>75.27</v>
       </c>
-      <c r="M50" s="23">
+      <c r="M50" s="20">
         <v>3.4279999999999999</v>
       </c>
-      <c r="N50" s="23">
+      <c r="N50" s="20">
         <v>0.113</v>
       </c>
-      <c r="O50" s="23" t="s">
+      <c r="O50" s="20" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2231,30 +2231,30 @@
       <c r="A53" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E53" s="13" t="s">
+      <c r="E53" s="10" t="s">
         <v>31</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
-      <c r="H53" s="8" t="s">
+      <c r="H53" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I53" s="8" t="s">
+      <c r="I53" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J53" s="8" t="s">
+      <c r="J53" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K53" s="13" t="s">
+      <c r="K53" s="10" t="s">
         <v>31</v>
       </c>
       <c r="L53" s="2"/>
@@ -2272,7 +2272,7 @@
       <c r="D54" s="5">
         <v>22</v>
       </c>
-      <c r="E54" s="15"/>
+      <c r="E54" s="12"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="5">
@@ -2284,7 +2284,7 @@
       <c r="J54" s="5">
         <v>771</v>
       </c>
-      <c r="K54" s="14" t="s">
+      <c r="K54" s="11" t="s">
         <v>54</v>
       </c>
       <c r="L54" s="2"/>
@@ -2311,35 +2311,35 @@
       <c r="A56" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D56" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E56" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F56" s="13" t="s">
+      <c r="F56" s="10" t="s">
         <v>31</v>
       </c>
       <c r="G56" s="2"/>
-      <c r="H56" s="8" t="s">
+      <c r="H56" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I56" s="8" t="s">
+      <c r="I56" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J56" s="8" t="s">
+      <c r="J56" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K56" s="8" t="s">
+      <c r="K56" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L56" s="13" t="s">
+      <c r="L56" s="10" t="s">
         <v>31</v>
       </c>
       <c r="M56" s="2"/>
@@ -2359,7 +2359,7 @@
       <c r="E57" s="5">
         <v>18</v>
       </c>
-      <c r="F57" s="15"/>
+      <c r="F57" s="12"/>
       <c r="G57" s="2"/>
       <c r="H57" s="5">
         <v>61</v>
@@ -2373,7 +2373,7 @@
       <c r="K57" s="5">
         <v>635</v>
       </c>
-      <c r="L57" s="14" t="s">
+      <c r="L57" s="11" t="s">
         <v>53</v>
       </c>
       <c r="M57" s="2"/>
@@ -2399,30 +2399,30 @@
       <c r="A59" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C59" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D59" s="8" t="s">
+      <c r="D59" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E59" s="13" t="s">
+      <c r="E59" s="10" t="s">
         <v>31</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
-      <c r="H59" s="8" t="s">
+      <c r="H59" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I59" s="8" t="s">
+      <c r="I59" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J59" s="8" t="s">
+      <c r="J59" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K59" s="13" t="s">
+      <c r="K59" s="10" t="s">
         <v>31</v>
       </c>
       <c r="L59" s="2"/>
@@ -2439,7 +2439,7 @@
       <c r="D60" s="5">
         <v>15</v>
       </c>
-      <c r="E60" s="15"/>
+      <c r="E60" s="12"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="5">
@@ -2451,7 +2451,7 @@
       <c r="J60" s="5">
         <v>541</v>
       </c>
-      <c r="K60" s="14" t="s">
+      <c r="K60" s="11" t="s">
         <v>52</v>
       </c>
       <c r="L60" s="2"/>
@@ -2475,68 +2475,68 @@
     </row>
     <row r="62" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="63" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="45" t="s">
+      <c r="B63" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C63" s="46"/>
-      <c r="D63" s="46"/>
-      <c r="E63" s="46"/>
-      <c r="F63" s="46"/>
-      <c r="G63" s="46"/>
-      <c r="H63" s="46"/>
-      <c r="I63" s="46"/>
-      <c r="J63" s="46"/>
-      <c r="K63" s="46"/>
-      <c r="L63" s="47"/>
-      <c r="M63" s="24" t="s">
+      <c r="C63" s="35"/>
+      <c r="D63" s="35"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="35"/>
+      <c r="G63" s="35"/>
+      <c r="H63" s="35"/>
+      <c r="I63" s="35"/>
+      <c r="J63" s="35"/>
+      <c r="K63" s="35"/>
+      <c r="L63" s="36"/>
+      <c r="M63" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="N63" s="25"/>
+      <c r="N63" s="38"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
-      <c r="H64" s="16"/>
-      <c r="I64" s="16"/>
-      <c r="J64" s="16"/>
-      <c r="K64" s="16"/>
-      <c r="L64" s="16"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="13"/>
+      <c r="K64" s="13"/>
+      <c r="L64" s="13"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E66" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="F66" s="30"/>
+      <c r="F66" s="29"/>
       <c r="H66" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="I66" s="29"/>
-      <c r="J66" s="35"/>
-      <c r="K66" s="34"/>
-      <c r="L66" s="34"/>
+      <c r="I66" s="30"/>
+      <c r="J66" s="27"/>
+      <c r="K66" s="26"/>
+      <c r="L66" s="26"/>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E67" s="7" t="s">
+      <c r="E67" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F67" s="7" t="s">
+      <c r="F67" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H67" s="7" t="s">
+      <c r="H67" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I67" s="7" t="s">
+      <c r="I67" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J67" s="26"/>
-      <c r="K67" s="26"/>
-      <c r="L67" s="26"/>
+      <c r="J67" s="21"/>
+      <c r="K67" s="21"/>
+      <c r="L67" s="21"/>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
     </row>
@@ -2547,14 +2547,14 @@
       <c r="E68" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F68" s="31">
+      <c r="F68" s="23">
         <v>0.6391</v>
       </c>
       <c r="G68" s="2"/>
       <c r="H68" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I68" s="27" t="s">
+      <c r="I68" s="22" t="s">
         <v>42</v>
       </c>
       <c r="J68" s="2"/>
@@ -2569,14 +2569,14 @@
       <c r="E69" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F69" s="31">
+      <c r="F69" s="23">
         <v>0.53779999999999994</v>
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I69" s="27" t="s">
+      <c r="I69" s="22" t="s">
         <v>47</v>
       </c>
       <c r="J69" s="2"/>
@@ -2591,14 +2591,14 @@
       <c r="E70" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F70" s="31">
+      <c r="F70" s="23">
         <v>0.81850000000000001</v>
       </c>
       <c r="G70" s="2"/>
       <c r="H70" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I70" s="27" t="s">
+      <c r="I70" s="22" t="s">
         <v>48</v>
       </c>
       <c r="J70" s="2"/>
@@ -2624,9 +2624,9 @@
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
-      <c r="D72" s="32"/>
-      <c r="E72" s="33"/>
-      <c r="F72" s="32"/>
+      <c r="D72" s="24"/>
+      <c r="E72" s="25"/>
+      <c r="F72" s="24"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
@@ -2638,14 +2638,14 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
-      <c r="B73" s="26"/>
-      <c r="C73" s="26"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="21"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="H73" s="2"/>
-      <c r="J73" s="26"/>
-      <c r="K73" s="26"/>
-      <c r="L73" s="26"/>
+      <c r="J73" s="21"/>
+      <c r="K73" s="21"/>
+      <c r="L73" s="21"/>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
     </row>
@@ -2662,27 +2662,27 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
-      <c r="B75" s="33"/>
-      <c r="C75" s="32"/>
+      <c r="B75" s="25"/>
+      <c r="C75" s="24"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
       <c r="H75" s="2"/>
-      <c r="J75" s="32"/>
-      <c r="K75" s="33"/>
-      <c r="L75" s="32"/>
+      <c r="J75" s="24"/>
+      <c r="K75" s="25"/>
+      <c r="L75" s="24"/>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
-      <c r="B76" s="26"/>
-      <c r="C76" s="26"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="21"/>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
       <c r="H76" s="2"/>
-      <c r="J76" s="26"/>
-      <c r="K76" s="26"/>
-      <c r="L76" s="26"/>
+      <c r="J76" s="21"/>
+      <c r="K76" s="21"/>
+      <c r="L76" s="21"/>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
     </row>
@@ -2699,27 +2699,27 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
-      <c r="B78" s="33"/>
-      <c r="C78" s="32"/>
+      <c r="B78" s="25"/>
+      <c r="C78" s="24"/>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
       <c r="H78" s="2"/>
-      <c r="J78" s="32"/>
-      <c r="K78" s="33"/>
-      <c r="L78" s="32"/>
+      <c r="J78" s="24"/>
+      <c r="K78" s="25"/>
+      <c r="L78" s="24"/>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
-      <c r="B79" s="26"/>
-      <c r="C79" s="26"/>
+      <c r="B79" s="21"/>
+      <c r="C79" s="21"/>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
       <c r="H79" s="2"/>
-      <c r="J79" s="26"/>
-      <c r="K79" s="26"/>
-      <c r="L79" s="26"/>
+      <c r="J79" s="21"/>
+      <c r="K79" s="21"/>
+      <c r="L79" s="21"/>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
     </row>
@@ -2735,6 +2735,15 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B43:L43"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="B22:L22"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="H25:L25"/>
+    <mergeCell ref="M25:O25"/>
     <mergeCell ref="E66:F66"/>
     <mergeCell ref="H66:I66"/>
     <mergeCell ref="B46:F46"/>
@@ -2742,15 +2751,6 @@
     <mergeCell ref="M46:O46"/>
     <mergeCell ref="B63:L63"/>
     <mergeCell ref="M63:N63"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="B22:L22"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="H25:L25"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="B43:L43"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="B1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>